<commit_message>
Season 14, matchdays prepares
</commit_message>
<xml_diff>
--- a/data/match_1.xlsx
+++ b/data/match_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton.shevchuk\dev\euroleague\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE32564-FF10-4CE7-BE83-0ACC8AC59FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DC885E-27AD-47F1-8447-D993B86FB05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="54">
   <si>
     <t>№</t>
   </si>
@@ -164,18 +164,12 @@
     <t>3:3</t>
   </si>
   <si>
-    <t>Фёдоров Михаил</t>
-  </si>
-  <si>
     <t>Муратов Игорь</t>
   </si>
   <si>
     <t>Гришин Антон</t>
   </si>
   <si>
-    <t>Оксанич Кирилл</t>
-  </si>
-  <si>
     <t>1:3</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>Титаренко Антон</t>
   </si>
   <si>
-    <t>Еременко Владислав</t>
-  </si>
-  <si>
     <t>Дробышев Артемий</t>
   </si>
   <si>
@@ -204,18 +195,35 @@
   </si>
   <si>
     <t>Махмудов Руслан</t>
+  </si>
+  <si>
+    <t>Зубатов Михаил</t>
+  </si>
+  <si>
+    <t>Котов Александр</t>
+  </si>
+  <si>
+    <t>2:3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -256,17 +264,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2 5" xfId="1" xr:uid="{19C298AE-AF7C-41EA-999B-123F97E378F7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,13 +576,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -647,67 +660,70 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>18</v>
+        <v>3.5</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -715,22 +731,22 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -748,37 +764,37 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -786,70 +802,70 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4" t="s">
         <v>23</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-      <c r="V4" t="s">
-        <v>32</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -860,52 +876,55 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
         <v>29</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>27</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -917,149 +936,84 @@
         <v>3</v>
       </c>
       <c r="V5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>15</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>51</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6" t="s">
-        <v>32</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1067,16 +1021,16 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1088,37 +1042,37 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -1137,71 +1091,66 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>12</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V9" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -1209,22 +1158,22 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>3.5</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1236,16 +1185,16 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" t="s">
         <v>27</v>
@@ -1254,25 +1203,25 @@
         <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1280,28 +1229,43 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
       <c r="I11">
         <v>0</v>
       </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
       <c r="K11">
         <v>0</v>
       </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
       <c r="M11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" t="s">
         <v>27</v>
@@ -1310,75 +1274,75 @@
         <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="R11" t="s">
+        <v>26</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
         <v>29</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12">
-        <v>2</v>
-      </c>
-      <c r="N12" t="s">
-        <v>27</v>
-      </c>
       <c r="O12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1390,13 +1354,13 @@
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="U12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1404,58 +1368,40 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>27</v>
-      </c>
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" t="s">
-        <v>26</v>
-      </c>
       <c r="M13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P13" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="Q13">
         <v>0</v>
-      </c>
-      <c r="R13" t="s">
-        <v>27</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -1546,37 +1492,37 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" t="s">
         <v>27</v>
@@ -1585,10 +1531,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="O15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P15" t="s">
         <v>26</v>
@@ -1597,10 +1543,10 @@
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T15" t="s">
         <v>26</v>
@@ -1609,7 +1555,7 @@
         <v>5</v>
       </c>
       <c r="V15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -1617,70 +1563,70 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>3.5</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
         <v>29</v>
       </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>27</v>
-      </c>
       <c r="O16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P16" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>35</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16">
+        <v>5</v>
+      </c>
+      <c r="V16" t="s">
         <v>32</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16">
-        <v>2</v>
-      </c>
-      <c r="T16" t="s">
-        <v>24</v>
-      </c>
-      <c r="U16">
-        <v>3</v>
-      </c>
-      <c r="V16" t="s">
-        <v>24</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -1688,13 +1634,13 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>3.5</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C17">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>28</v>
@@ -1703,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1715,10 +1661,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L17" t="s">
         <v>26</v>
@@ -1733,25 +1679,25 @@
         <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="S17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="U17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -1759,149 +1705,78 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C18">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
         <v>28</v>
       </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
-      <c r="L18" t="s">
-        <v>27</v>
-      </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="S18">
         <v>2</v>
       </c>
       <c r="T18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V18" t="s">
         <v>27</v>
       </c>
       <c r="W18">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19">
-        <v>2</v>
-      </c>
-      <c r="N19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19">
-        <v>3</v>
-      </c>
-      <c r="P19" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q19">
-        <v>3</v>
-      </c>
-      <c r="R19" t="s">
-        <v>26</v>
-      </c>
-      <c r="S19">
-        <v>2</v>
-      </c>
-      <c r="T19" t="s">
-        <v>24</v>
-      </c>
-      <c r="U19">
-        <v>3</v>
-      </c>
-      <c r="V19" t="s">
-        <v>29</v>
-      </c>
-      <c r="W19">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W19">
-    <sortCondition ref="C1:C19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W18">
+    <sortCondition ref="B1:B18"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>